<commit_message>
fixed bugs in performane view
</commit_message>
<xml_diff>
--- a/Project/functions/public/web4/examples/Assignment1.xlsx
+++ b/Project/functions/public/web4/examples/Assignment1.xlsx
@@ -19,19 +19,19 @@
     <t>Marks</t>
   </si>
   <si>
-    <t>Nirasha Sewwandi</t>
+    <t>W.A.T.N.Jayathilake</t>
   </si>
   <si>
     <t>30/30</t>
   </si>
   <si>
-    <t>Thakshila Nadeeshani</t>
+    <t>D.W.S.N.Sewwandi</t>
   </si>
   <si>
     <t>Not Completed</t>
   </si>
   <si>
-    <t>Mahela Bandara</t>
+    <t>L.R.M.U.BANDARA</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Evaluation report added for perf analysis
</commit_message>
<xml_diff>
--- a/Project/functions/public/web4/examples/Assignment1.xlsx
+++ b/Project/functions/public/web4/examples/Assignment1.xlsx
@@ -19,19 +19,19 @@
     <t>Marks</t>
   </si>
   <si>
-    <t>Nirasha Sewwandi</t>
+    <t>W.A.T.N.Jayathilake</t>
   </si>
   <si>
     <t>30/30</t>
   </si>
   <si>
-    <t>Thakshila Nadeeshani</t>
+    <t>D.W.S.N.Sewwandi</t>
   </si>
   <si>
     <t>Not Completed</t>
   </si>
   <si>
-    <t>Mahela Bandara</t>
+    <t>L.R.M.U.BANDARA</t>
   </si>
 </sst>
 </file>

</xml_diff>